<commit_message>
added data to wattHour graphs
</commit_message>
<xml_diff>
--- a/data/wattHours_to_time/non_resistive.xlsx
+++ b/data/wattHours_to_time/non_resistive.xlsx
@@ -11,15 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>PLM Start</t>
   </si>
@@ -43,6 +40,12 @@
   </si>
   <si>
     <t>PB Error</t>
+  </si>
+  <si>
+    <t>KW</t>
+  </si>
+  <si>
+    <t>KW Error</t>
   </si>
 </sst>
 </file>
@@ -112,16 +115,14 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$5:$A$45</c:f>
@@ -200,16 +201,14 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$5:$A$45</c:f>
@@ -288,7 +287,87 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$5:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -298,11 +377,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="62072704"/>
-        <c:axId val="57855360"/>
+        <c:axId val="46678016"/>
+        <c:axId val="46679552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62072704"/>
+        <c:axId val="46678016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -312,12 +391,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57855360"/>
+        <c:crossAx val="46679552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57855360"/>
+        <c:axId val="46679552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -328,7 +407,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62072704"/>
+        <c:crossAx val="46678016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -383,134 +462,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="A5">
-            <v>0</v>
-          </cell>
-          <cell r="D5">
-            <v>0</v>
-          </cell>
-          <cell r="E5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>2</v>
-          </cell>
-          <cell r="D6">
-            <v>8.9500000000000455</v>
-          </cell>
-          <cell r="E6">
-            <v>9.8699999999999992</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>4</v>
-          </cell>
-          <cell r="D7">
-            <v>17.300000000000011</v>
-          </cell>
-          <cell r="E7">
-            <v>18.78</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>10</v>
-          </cell>
-          <cell r="D8">
-            <v>42.700000000000045</v>
-          </cell>
-          <cell r="E8">
-            <v>44.69</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>20</v>
-          </cell>
-          <cell r="D9">
-            <v>84.150000000000034</v>
-          </cell>
-          <cell r="E9">
-            <v>88.75</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>40</v>
-          </cell>
-          <cell r="D10">
-            <v>167.66000000000003</v>
-          </cell>
-          <cell r="E10">
-            <v>182.65</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>60</v>
-          </cell>
-          <cell r="D11">
-            <v>251.77000000000004</v>
-          </cell>
-          <cell r="E11">
-            <v>274.10000000000002</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>80</v>
-          </cell>
-          <cell r="D12">
-            <v>335.50000000000006</v>
-          </cell>
-          <cell r="E12">
-            <v>365.13</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>100</v>
-          </cell>
-          <cell r="D13">
-            <v>419.36000000000007</v>
-          </cell>
-          <cell r="E13">
-            <v>456.46</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>120</v>
-          </cell>
-          <cell r="D14">
-            <v>503.82</v>
-          </cell>
-          <cell r="E14">
-            <v>548.55999999999995</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -800,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +762,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +770,7 @@
         <v>938.75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -827,7 +778,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -846,8 +797,14 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -858,18 +815,24 @@
         <v>0.2</v>
       </c>
       <c r="D5">
-        <f>B5-B$1</f>
+        <f t="shared" ref="D5:D14" si="0">B5-B$1</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>C5-B$2</f>
+        <f t="shared" ref="E5:E14" si="1">C5-B$2</f>
         <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -880,19 +843,23 @@
         <v>1.74</v>
       </c>
       <c r="D6">
-        <f>B6-B$1</f>
+        <f t="shared" si="0"/>
         <v>1.5800000000000409</v>
       </c>
       <c r="E6">
-        <f>C6-B$2</f>
+        <f t="shared" si="1"/>
         <v>1.54</v>
       </c>
       <c r="F6">
-        <f>ABS(E6-D6)/D6*100</f>
+        <f t="shared" ref="F6:F14" si="2">ABS(E6-D6)/D6*100</f>
         <v>2.5316455696227758</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f>ABS(G6-D6)/D6*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -903,19 +870,23 @@
         <v>3.33</v>
       </c>
       <c r="D7">
-        <f>B7-B$1</f>
+        <f t="shared" si="0"/>
         <v>3.07000000000005</v>
       </c>
       <c r="E7">
-        <f>C7-B$2</f>
+        <f t="shared" si="1"/>
         <v>3.13</v>
       </c>
       <c r="F7">
-        <f>ABS(E7-D7)/D7*100</f>
+        <f t="shared" si="2"/>
         <v>1.9543973941351429</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" ref="H7:H14" si="3">ABS(G7-D7)/D7*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -926,19 +897,26 @@
         <v>8.07</v>
       </c>
       <c r="D8">
-        <f>B8-B$1</f>
+        <f t="shared" si="0"/>
         <v>7.3700000000000045</v>
       </c>
       <c r="E8">
-        <f>C8-B$2</f>
+        <f t="shared" si="1"/>
         <v>7.87</v>
       </c>
       <c r="F8">
-        <f>ABS(E8-D8)/D8*100</f>
+        <f t="shared" si="2"/>
         <v>6.7842605156037354</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20</v>
       </c>
@@ -949,19 +927,26 @@
         <v>16.11</v>
       </c>
       <c r="D9">
-        <f>B9-B$1</f>
+        <f t="shared" si="0"/>
         <v>14.590000000000032</v>
       </c>
       <c r="E9">
-        <f>C9-B$2</f>
+        <f t="shared" si="1"/>
         <v>15.91</v>
       </c>
       <c r="F9">
-        <f>ABS(E9-D9)/D9*100</f>
+        <f t="shared" si="2"/>
         <v>9.0472926662094952</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>31.459904043865812</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -972,19 +957,26 @@
         <v>32.450000000000003</v>
       </c>
       <c r="D10">
-        <f>B10-B$1</f>
+        <f t="shared" si="0"/>
         <v>29.470000000000027</v>
       </c>
       <c r="E10">
-        <f>C10-B$2</f>
+        <f t="shared" si="1"/>
         <v>32.25</v>
       </c>
       <c r="F10">
-        <f>ABS(E10-D10)/D10*100</f>
+        <f t="shared" si="2"/>
         <v>9.4333220223955561</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>32.134373939599655</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>60</v>
       </c>
@@ -995,19 +987,26 @@
         <v>48.79</v>
       </c>
       <c r="D11">
-        <f>B11-B$1</f>
+        <f t="shared" si="0"/>
         <v>44.309999999999945</v>
       </c>
       <c r="E11">
-        <f>C11-B$2</f>
+        <f t="shared" si="1"/>
         <v>48.589999999999996</v>
       </c>
       <c r="F11">
-        <f>ABS(E11-D11)/D11*100</f>
+        <f t="shared" si="2"/>
         <v>9.6592191378922507</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>40</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>9.7269239449333114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>80</v>
       </c>
@@ -1018,19 +1017,26 @@
         <v>65.28</v>
       </c>
       <c r="D12">
-        <f>B12-B$1</f>
+        <f t="shared" si="0"/>
         <v>59.230000000000018</v>
       </c>
       <c r="E12">
-        <f>C12-B$2</f>
+        <f t="shared" si="1"/>
         <v>65.08</v>
       </c>
       <c r="F12">
-        <f>ABS(E12-D12)/D12*100</f>
+        <f t="shared" si="2"/>
         <v>9.8767516461252391</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>15.583319263886569</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>100</v>
       </c>
@@ -1041,19 +1047,26 @@
         <v>81.42</v>
       </c>
       <c r="D13">
-        <f>B13-B$1</f>
+        <f t="shared" si="0"/>
         <v>73.919999999999959</v>
       </c>
       <c r="E13">
-        <f>C13-B$2</f>
+        <f t="shared" si="1"/>
         <v>81.22</v>
       </c>
       <c r="F13">
-        <f>ABS(E13-D13)/D13*100</f>
+        <f t="shared" si="2"/>
         <v>9.8755411255411847</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>70</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>5.3030303030302504</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>120</v>
       </c>
@@ -1064,16 +1077,23 @@
         <v>97.75</v>
       </c>
       <c r="D14">
-        <f>B14-B$1</f>
+        <f t="shared" si="0"/>
         <v>88.839999999999918</v>
       </c>
       <c r="E14">
-        <f>C14-B$2</f>
+        <f t="shared" si="1"/>
         <v>97.55</v>
       </c>
       <c r="F14">
-        <f>ABS(E14-D14)/D14*100</f>
+        <f t="shared" si="2"/>
         <v>9.8041422782531384</v>
+      </c>
+      <c r="G14">
+        <v>80</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>9.9504727600179272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added watts up to non resistive watt hours data
</commit_message>
<xml_diff>
--- a/data/wattHours_to_time/non_resistive.xlsx
+++ b/data/wattHours_to_time/non_resistive.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>PLM Start</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>KW Error</t>
+  </si>
+  <si>
+    <t>WU</t>
+  </si>
+  <si>
+    <t>WU Error</t>
   </si>
 </sst>
 </file>
@@ -125,10 +131,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$45</c:f>
+              <c:f>Sheet1!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -164,10 +170,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$45</c:f>
+              <c:f>Sheet1!$D$5:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -211,10 +217,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$5:$A$45</c:f>
+              <c:f>Sheet1!$A$5:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -250,10 +256,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$45</c:f>
+              <c:f>Sheet1!$E$5:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -369,6 +375,92 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$5:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>65.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -377,11 +469,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="46678016"/>
-        <c:axId val="46679552"/>
+        <c:axId val="131723648"/>
+        <c:axId val="131725184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46678016"/>
+        <c:axId val="131723648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,12 +483,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46679552"/>
+        <c:crossAx val="131725184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46679552"/>
+        <c:axId val="131725184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,7 +499,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46678016"/>
+        <c:crossAx val="131723648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -751,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +854,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +862,7 @@
         <v>938.75</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -778,7 +870,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -803,8 +895,14 @@
       <c r="H4" t="s">
         <v>9</v>
       </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -831,8 +929,14 @@
       <c r="H5">
         <v>0</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -858,8 +962,15 @@
         <f>ABS(G6-D6)/D6*100</f>
         <v>100</v>
       </c>
+      <c r="I6">
+        <v>1.7</v>
+      </c>
+      <c r="J6">
+        <f>ABS(I6-D6)/D6*100</f>
+        <v>7.5949367088579702</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -885,8 +996,15 @@
         <f t="shared" ref="H7:H14" si="3">ABS(G7-D7)/D7*100</f>
         <v>100</v>
       </c>
+      <c r="I7">
+        <v>3.4</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:J14" si="4">ABS(I7-D7)/D7*100</f>
+        <v>10.749185667750636</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -915,8 +1033,15 @@
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
+      <c r="I8">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>12.618724559023006</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20</v>
       </c>
@@ -945,8 +1070,15 @@
         <f t="shared" si="3"/>
         <v>31.459904043865812</v>
       </c>
+      <c r="I9">
+        <v>16.5</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>13.091158327621413</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -975,8 +1107,15 @@
         <f t="shared" si="3"/>
         <v>32.134373939599655</v>
       </c>
+      <c r="I10">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>10.960298608754572</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>60</v>
       </c>
@@ -1005,8 +1144,15 @@
         <f t="shared" si="3"/>
         <v>9.7269239449333114</v>
       </c>
+      <c r="I11">
+        <v>49.1</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>10.810200857594362</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>80</v>
       </c>
@@ -1035,8 +1181,15 @@
         <f t="shared" si="3"/>
         <v>15.583319263886569</v>
       </c>
+      <c r="I12">
+        <v>65.7</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>10.923518487253052</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>100</v>
       </c>
@@ -1065,8 +1218,15 @@
         <f t="shared" si="3"/>
         <v>5.3030303030302504</v>
       </c>
+      <c r="I13">
+        <v>82</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>10.930735930735992</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>120</v>
       </c>
@@ -1094,6 +1254,13 @@
       <c r="H14">
         <f t="shared" si="3"/>
         <v>9.9504727600179272</v>
+      </c>
+      <c r="I14">
+        <v>99.2</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>11.661413777577774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>